<commit_message>
revisi final tanggal 21/02.2023
</commit_message>
<xml_diff>
--- a/DAS POWER/List Komponen Das Power.xlsx
+++ b/DAS POWER/List Komponen Das Power.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\MGI\DAS POWER\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\MGI\DAS POWER\PT.MGI-DAS-POWER\DAS POWER\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
   <si>
     <t>No</t>
   </si>
@@ -245,9 +245,6 @@
     <t>hall efect sensor for DC current measuring 100A</t>
   </si>
   <si>
-    <t>https://www.tokopedia.com/fadalstore/d-c2t-hall-efect-sensor-for-dc-current-measuring-100a-200a-fathor-d-c2t-100a</t>
-  </si>
-  <si>
     <t>https://www.tokopedia.com/gst-21/konektor-molex-2-3-4-5-6-pin-soket-socket-molek-pitch-2-5-ph-jst-xh-4-pin?extParam=ivf%3Dfalse%26src%3Dsearch</t>
   </si>
   <si>
@@ -267,6 +264,33 @@
   </si>
   <si>
     <t>segera diorder</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/fadalstore/ankerui-ahkc-eka-0-100-a-5v-20-hall-open-type-current-sensor</t>
+  </si>
+  <si>
+    <t>Beli 3 dan Segera diorder karena pre-order</t>
+  </si>
+  <si>
+    <t>2. Belum Termasuk Box</t>
+  </si>
+  <si>
+    <t>terminal block hijau 9p</t>
+  </si>
+  <si>
+    <t>https://www.tokopedia.com/s3-satriasecure/l-siku-pluggable-9-p-pin-terminal-blok-9p-9pin-screw-plugable-block</t>
+  </si>
+  <si>
+    <t>Komponen Embbed di China</t>
+  </si>
+  <si>
+    <t>Komponen yang sudah embbed di china(TIDAK PERLU DIORDER)</t>
+  </si>
+  <si>
+    <t>TIDAK PERLU DIORDER</t>
+  </si>
+  <si>
+    <t>KEPERLUAN DAS POWER UNTUK 1 UNIT</t>
   </si>
 </sst>
 </file>
@@ -293,7 +317,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,8 +354,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -354,12 +390,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -373,38 +455,67 @@
     <xf numFmtId="42" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -686,10 +797,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G39" sqref="G39"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -698,729 +809,720 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="142.6640625" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.77734375" customWidth="1"/>
+    <col min="8" max="8" width="142.6640625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="9" t="s">
+      <c r="H2" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
+    <row r="3" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="15">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="15">
         <v>2</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D3" s="16">
         <v>500</v>
       </c>
-      <c r="E2" s="2">
+      <c r="E3" s="16">
         <v>7000</v>
       </c>
-      <c r="F2" s="2">
-        <f>(C2*D2)+E2</f>
+      <c r="F3" s="16">
+        <f>(C3*D3)+E3</f>
         <v>8000</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="10" t="s">
+      <c r="G3" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="H3" s="17" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="1">
+    <row r="4" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="15">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C4" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D4" s="16">
         <v>6000</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E4" s="16">
         <v>7000</v>
       </c>
-      <c r="F3" s="2">
-        <f t="shared" ref="F3:F35" si="0">(C3*D3)+E3</f>
+      <c r="F4" s="16">
+        <f t="shared" ref="F4:F37" si="0">(C4*D4)+E4</f>
         <v>13000</v>
       </c>
-      <c r="G3" s="1"/>
-      <c r="H3" s="10" t="s">
+      <c r="G4" s="27"/>
+      <c r="H4" s="17" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
+    <row r="5" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C5" s="15">
         <v>10</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D5" s="16">
         <v>100</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2">
+      <c r="E5" s="16"/>
+      <c r="F5" s="16">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G4" s="1"/>
-      <c r="H4" s="10" t="s">
+      <c r="G5" s="27"/>
+      <c r="H5" s="17" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
+    <row r="6" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C6" s="15">
         <v>2</v>
       </c>
-      <c r="D5" s="2">
+      <c r="D6" s="16">
         <v>1000</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2">
+      <c r="E6" s="16"/>
+      <c r="F6" s="16">
         <f t="shared" si="0"/>
         <v>2000</v>
       </c>
-      <c r="G5" s="1"/>
-      <c r="H5" s="10" t="s">
+      <c r="G6" s="27"/>
+      <c r="H6" s="17" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
+    <row r="7" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="15">
         <v>5</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B7" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C7" s="15">
         <v>8</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D7" s="16">
         <v>100</v>
       </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2">
+      <c r="E7" s="16"/>
+      <c r="F7" s="16">
         <f t="shared" si="0"/>
         <v>800</v>
       </c>
-      <c r="G6" s="1"/>
-      <c r="H6" s="10" t="s">
+      <c r="G7" s="27"/>
+      <c r="H7" s="17" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
+    <row r="8" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="15">
         <v>6</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C8" s="15">
         <v>3</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D8" s="16">
         <v>1000</v>
       </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2">
+      <c r="E8" s="16"/>
+      <c r="F8" s="16">
         <f t="shared" si="0"/>
         <v>3000</v>
       </c>
-      <c r="G7" s="1"/>
-      <c r="H7" s="10" t="s">
+      <c r="G8" s="27"/>
+      <c r="H8" s="17" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
+    <row r="9" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="15">
         <v>7</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C9" s="15">
         <v>1</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D9" s="16">
         <v>3050</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E9" s="16">
         <v>7000</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F9" s="16">
         <f t="shared" si="0"/>
         <v>10050</v>
       </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="10" t="s">
+      <c r="G9" s="27"/>
+      <c r="H9" s="17" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
+    <row r="10" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="15">
         <v>8</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B10" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C10" s="15">
         <v>5</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D10" s="16">
         <v>220</v>
       </c>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2">
+      <c r="E10" s="16"/>
+      <c r="F10" s="16">
         <f t="shared" si="0"/>
         <v>1100</v>
       </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="10" t="s">
+      <c r="G10" s="27"/>
+      <c r="H10" s="17" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
+    <row r="11" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="15">
         <v>9</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B11" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C11" s="15">
         <v>8</v>
       </c>
-      <c r="D10" s="2">
+      <c r="D11" s="16">
         <v>300</v>
       </c>
-      <c r="E10" s="2">
+      <c r="E11" s="16">
         <v>16000</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F11" s="16">
         <f t="shared" si="0"/>
         <v>18400</v>
       </c>
-      <c r="G10" s="1"/>
-      <c r="H10" s="10" t="s">
+      <c r="G11" s="27"/>
+      <c r="H11" s="17" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" s="1">
+    <row r="12" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="15">
         <v>10</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="B12" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C12" s="15">
         <v>2</v>
       </c>
-      <c r="D11" s="2">
+      <c r="D12" s="16">
         <v>800</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2">
+      <c r="E12" s="16"/>
+      <c r="F12" s="16">
         <f t="shared" si="0"/>
         <v>1600</v>
       </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="10" t="s">
+      <c r="G12" s="27"/>
+      <c r="H12" s="17" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" s="1">
+    <row r="13" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15">
         <v>11</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B13" s="15" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C13" s="15">
         <v>10</v>
       </c>
-      <c r="D12" s="2">
+      <c r="D13" s="16">
         <v>1000</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2">
+      <c r="E13" s="16"/>
+      <c r="F13" s="16">
         <f t="shared" si="0"/>
         <v>10000</v>
       </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="10" t="s">
+      <c r="G13" s="27"/>
+      <c r="H13" s="17" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" s="1">
+    <row r="14" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15">
         <v>12</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B14" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C14" s="15">
         <v>10</v>
       </c>
-      <c r="D13" s="2">
+      <c r="D14" s="16">
         <v>3000</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E14" s="16">
         <v>13000</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F14" s="16">
         <f t="shared" si="0"/>
         <v>43000</v>
       </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="10" t="s">
+      <c r="G14" s="27"/>
+      <c r="H14" s="17" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" s="1">
+    <row r="15" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
         <v>13</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B15" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C15" s="15">
         <v>8</v>
       </c>
-      <c r="D14" s="2">
+      <c r="D15" s="16">
         <v>600</v>
       </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2">
+      <c r="E15" s="16"/>
+      <c r="F15" s="16">
         <f t="shared" si="0"/>
         <v>4800</v>
       </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="10" t="s">
+      <c r="G15" s="27"/>
+      <c r="H15" s="17" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" s="1">
+    <row r="16" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15">
         <v>14</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B16" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C16" s="15">
         <v>8</v>
       </c>
-      <c r="D15" s="2">
+      <c r="D16" s="16">
         <v>500</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2">
+      <c r="E16" s="16"/>
+      <c r="F16" s="16">
         <f t="shared" si="0"/>
         <v>4000</v>
       </c>
-      <c r="G15" s="1"/>
-      <c r="H15" s="10" t="s">
+      <c r="G16" s="27"/>
+      <c r="H16" s="17" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" s="1">
+    <row r="17" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="15">
         <v>15</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B17" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C17" s="15">
         <v>5</v>
       </c>
-      <c r="D16" s="2">
+      <c r="D17" s="16">
         <v>100</v>
       </c>
-      <c r="E16" s="2">
+      <c r="E17" s="16">
         <v>12000</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F17" s="16">
         <f t="shared" si="0"/>
         <v>12500</v>
       </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="10" t="s">
+      <c r="G17" s="27"/>
+      <c r="H17" s="17" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" s="1">
+    <row r="18" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="15">
         <v>16</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B18" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C18" s="15">
         <v>5</v>
       </c>
-      <c r="D17" s="2">
+      <c r="D18" s="16">
         <v>200</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2">
+      <c r="E18" s="16"/>
+      <c r="F18" s="16">
         <f t="shared" si="0"/>
         <v>1000</v>
       </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="10" t="s">
+      <c r="G18" s="27"/>
+      <c r="H18" s="17" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" s="1">
+    <row r="19" spans="1:8" s="23" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
         <v>17</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B19" s="19" t="s">
         <v>26</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C19" s="19">
         <v>3</v>
       </c>
-      <c r="D18" s="2">
+      <c r="D19" s="20">
         <v>15000</v>
       </c>
-      <c r="E18" s="2">
+      <c r="E19" s="20">
         <v>7000</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F19" s="20">
         <f t="shared" si="0"/>
         <v>52000</v>
       </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="10" t="s">
+      <c r="G19" s="21"/>
+      <c r="H19" s="22" t="s">
         <v>27</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" s="1">
-        <v>18</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C19" s="1">
-        <v>1</v>
-      </c>
-      <c r="D19" s="2">
-        <v>15000</v>
-      </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2">
-        <f t="shared" si="0"/>
-        <v>15000</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="10" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="C20" s="1">
         <v>1</v>
       </c>
       <c r="D20" s="2">
-        <v>80000</v>
+        <v>15000</v>
       </c>
       <c r="E20" s="2"/>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>80000</v>
+        <v>15000</v>
       </c>
       <c r="G20" s="1"/>
-      <c r="H20" s="10" t="s">
-        <v>44</v>
+      <c r="H20" s="7" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D21" s="2">
-        <v>150000</v>
+        <v>80000</v>
       </c>
       <c r="E21" s="2"/>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>450000</v>
+        <v>80000</v>
       </c>
       <c r="G21" s="1"/>
-      <c r="H21" s="10" t="s">
-        <v>46</v>
+      <c r="H21" s="7" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1">
         <v>3</v>
       </c>
       <c r="D22" s="2">
-        <v>80000</v>
+        <v>150000</v>
       </c>
       <c r="E22" s="2"/>
       <c r="F22" s="2">
         <f t="shared" si="0"/>
+        <v>450000</v>
+      </c>
+      <c r="G22" s="1"/>
+      <c r="H22" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C23" s="1">
+        <v>3</v>
+      </c>
+      <c r="D23" s="2">
+        <v>80000</v>
+      </c>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2">
+        <f t="shared" si="0"/>
         <v>240000</v>
       </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="10" t="s">
+      <c r="G23" s="1"/>
+      <c r="H23" s="7" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="7">
+    <row r="24" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="5">
         <v>22</v>
       </c>
-      <c r="B23" s="7" t="s">
+      <c r="B24" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C24" s="5">
         <v>1</v>
       </c>
-      <c r="D23" s="8">
+      <c r="D24" s="6">
         <v>70000</v>
       </c>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8">
+      <c r="E24" s="6"/>
+      <c r="F24" s="6">
         <f t="shared" si="0"/>
         <v>70000</v>
       </c>
-      <c r="G23" s="7" t="s">
+      <c r="G24" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H24" s="11" t="s">
         <v>68</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" s="1">
-        <v>23</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C24" s="1">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
-        <v>9600</v>
-      </c>
-      <c r="E24" s="2">
-        <v>20000</v>
-      </c>
-      <c r="F24" s="2">
-        <f t="shared" si="0"/>
-        <v>48800</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="10" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C25" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" s="2">
-        <v>3600</v>
-      </c>
-      <c r="E25" s="2"/>
+        <v>9600</v>
+      </c>
+      <c r="E25" s="2">
+        <v>20000</v>
+      </c>
       <c r="F25" s="2">
         <f t="shared" si="0"/>
-        <v>21600</v>
+        <v>39200</v>
       </c>
       <c r="G25" s="1"/>
-      <c r="H25" s="10" t="s">
-        <v>57</v>
+      <c r="H25" s="7" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C26" s="1">
-        <v>2</v>
-      </c>
-      <c r="D26" s="2"/>
+        <v>6</v>
+      </c>
+      <c r="D26" s="2">
+        <v>3600</v>
+      </c>
       <c r="E26" s="2"/>
       <c r="F26" s="2">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>21600</v>
       </c>
       <c r="G26" s="1"/>
-      <c r="H26" s="11"/>
+      <c r="H26" s="7" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>41</v>
+        <v>83</v>
       </c>
       <c r="C27" s="1">
         <v>1</v>
       </c>
       <c r="D27" s="2">
-        <v>39000</v>
-      </c>
-      <c r="E27" s="2">
-        <v>21000</v>
-      </c>
+        <v>12700</v>
+      </c>
+      <c r="E27" s="2"/>
       <c r="F27" s="2">
         <f t="shared" si="0"/>
-        <v>60000</v>
+        <v>12700</v>
       </c>
       <c r="G27" s="1"/>
-      <c r="H27" s="10" t="s">
-        <v>42</v>
+      <c r="H27" s="7" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G28" s="1"/>
+      <c r="H28" s="8"/>
+    </row>
+    <row r="29" spans="1:8" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="15">
         <v>27</v>
       </c>
-      <c r="B28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="C28" s="1">
+      <c r="B29" s="15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C29" s="15">
         <v>1</v>
       </c>
-      <c r="D28" s="2">
+      <c r="D29" s="16">
+        <v>39000</v>
+      </c>
+      <c r="E29" s="16">
         <v>21000</v>
       </c>
-      <c r="E28" s="2">
-        <v>7000</v>
-      </c>
-      <c r="F28" s="2">
-        <f t="shared" si="0"/>
-        <v>28000</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="10" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" s="1">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="C29" s="1">
-        <v>1</v>
-      </c>
-      <c r="D29" s="2">
-        <v>1200</v>
-      </c>
-      <c r="E29" s="2">
-        <v>10000</v>
-      </c>
-      <c r="F29" s="2">
-        <f t="shared" si="0"/>
-        <v>11200</v>
-      </c>
-      <c r="G29" s="1"/>
-      <c r="H29" s="10" t="s">
-        <v>62</v>
+      <c r="F29" s="16">
+        <f t="shared" si="0"/>
+        <v>60000</v>
+      </c>
+      <c r="G29" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="H29" s="17" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>70</v>
       </c>
       <c r="C30" s="1">
         <v>1</v>
       </c>
       <c r="D30" s="2">
-        <v>1200</v>
-      </c>
-      <c r="E30" s="2"/>
+        <v>21000</v>
+      </c>
+      <c r="E30" s="2">
+        <v>7000</v>
+      </c>
       <c r="F30" s="2">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>28000</v>
       </c>
       <c r="G30" s="1"/>
-      <c r="H30" s="10" t="s">
-        <v>63</v>
+      <c r="H30" s="7" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C31" s="1">
         <v>1</v>
@@ -1428,22 +1530,24 @@
       <c r="D31" s="2">
         <v>1200</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="2">
+        <v>10000</v>
+      </c>
       <c r="F31" s="2">
         <f t="shared" si="0"/>
-        <v>1200</v>
+        <v>11200</v>
       </c>
       <c r="G31" s="1"/>
-      <c r="H31" s="10" t="s">
-        <v>64</v>
+      <c r="H31" s="7" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" s="1">
         <v>1</v>
@@ -1457,149 +1561,215 @@
         <v>1200</v>
       </c>
       <c r="G32" s="1"/>
-      <c r="H32" s="10" t="s">
-        <v>65</v>
+      <c r="H32" s="7" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
+        <v>31</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="1">
+        <v>1</v>
+      </c>
+      <c r="D33" s="2">
+        <v>1200</v>
+      </c>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G33" s="1"/>
+      <c r="H33" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" s="1">
         <v>32</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B34" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C34" s="1">
+        <v>1</v>
+      </c>
+      <c r="D34" s="2">
+        <v>1200</v>
+      </c>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2">
+        <f t="shared" si="0"/>
+        <v>1200</v>
+      </c>
+      <c r="G34" s="1"/>
+      <c r="H34" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" s="1">
+        <v>33</v>
+      </c>
+      <c r="B35" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C35" s="1">
         <v>2</v>
       </c>
-      <c r="D33" s="2">
+      <c r="D35" s="2">
         <v>1600</v>
       </c>
-      <c r="E33" s="2">
+      <c r="E35" s="2">
         <v>7000</v>
       </c>
-      <c r="F33" s="2">
+      <c r="F35" s="2">
         <f t="shared" si="0"/>
         <v>10200</v>
       </c>
-      <c r="G33" s="1"/>
-      <c r="H33" s="10" t="s">
+      <c r="G35" s="1"/>
+      <c r="H35" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" s="12" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36" s="5">
+        <v>34</v>
+      </c>
+      <c r="B36" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="5">
+        <v>3</v>
+      </c>
+      <c r="D36" s="6">
+        <v>440000</v>
+      </c>
+      <c r="E36" s="6">
+        <v>25000</v>
+      </c>
+      <c r="F36" s="6">
+        <f t="shared" si="0"/>
+        <v>1345000</v>
+      </c>
+      <c r="G36" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="5">
+        <v>35</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="5">
+        <v>1</v>
+      </c>
+      <c r="D37" s="6">
+        <v>38000</v>
+      </c>
+      <c r="E37" s="6">
+        <v>10000</v>
+      </c>
+      <c r="F37" s="6">
+        <f t="shared" si="0"/>
+        <v>48000</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="B38" s="24"/>
+      <c r="C38" s="24"/>
+      <c r="D38" s="24"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="4">
+        <f>SUM(F3:F37)</f>
+        <v>2620750</v>
+      </c>
+      <c r="G38" s="1"/>
+      <c r="H38" s="8"/>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" s="13" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="1">
-        <v>33</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="C34" s="1">
-        <v>3</v>
-      </c>
-      <c r="D34" s="2">
-        <v>455000</v>
-      </c>
-      <c r="E34" s="2">
-        <v>25000</v>
-      </c>
-      <c r="F34" s="2">
-        <f t="shared" si="0"/>
-        <v>1390000</v>
-      </c>
-      <c r="G34" s="1"/>
-      <c r="H34" s="10" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="7">
-        <v>34</v>
-      </c>
-      <c r="B35" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="C35" s="7">
-        <v>1</v>
-      </c>
-      <c r="D35" s="8">
-        <v>38000</v>
-      </c>
-      <c r="E35" s="8">
-        <v>10000</v>
-      </c>
-      <c r="F35" s="8">
-        <f t="shared" si="0"/>
-        <v>48000</v>
-      </c>
-      <c r="G35" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="H35" s="14" t="s">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" s="13" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="4">
-        <f>SUM(F2:F34)</f>
-        <v>2614650</v>
-      </c>
-      <c r="G36" s="1"/>
-      <c r="H36" s="11"/>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" s="16" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" s="16" t="s">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" s="12"/>
+      <c r="B48" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" s="15"/>
-      <c r="B46" t="s">
-        <v>80</v>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A49" s="18"/>
+      <c r="B49" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A36:E36"/>
+  <mergeCells count="3">
+    <mergeCell ref="A38:E38"/>
+    <mergeCell ref="G3:G18"/>
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1"/>
-    <hyperlink ref="H3" r:id="rId2"/>
-    <hyperlink ref="H8" r:id="rId3"/>
-    <hyperlink ref="H9" r:id="rId4"/>
-    <hyperlink ref="H10" r:id="rId5"/>
-    <hyperlink ref="H11" r:id="rId6"/>
-    <hyperlink ref="H14" r:id="rId7"/>
-    <hyperlink ref="H16" r:id="rId8"/>
-    <hyperlink ref="H18" r:id="rId9"/>
-    <hyperlink ref="H19" r:id="rId10"/>
-    <hyperlink ref="H17" r:id="rId11"/>
-    <hyperlink ref="H5" r:id="rId12"/>
-    <hyperlink ref="H6" r:id="rId13"/>
-    <hyperlink ref="H7" r:id="rId14"/>
-    <hyperlink ref="H20" r:id="rId15"/>
-    <hyperlink ref="H27" r:id="rId16"/>
-    <hyperlink ref="H24" r:id="rId17"/>
-    <hyperlink ref="H25" r:id="rId18"/>
-    <hyperlink ref="H34" r:id="rId19"/>
+    <hyperlink ref="H3" r:id="rId1"/>
+    <hyperlink ref="H4" r:id="rId2"/>
+    <hyperlink ref="H9" r:id="rId3"/>
+    <hyperlink ref="H10" r:id="rId4"/>
+    <hyperlink ref="H11" r:id="rId5"/>
+    <hyperlink ref="H12" r:id="rId6"/>
+    <hyperlink ref="H15" r:id="rId7"/>
+    <hyperlink ref="H17" r:id="rId8"/>
+    <hyperlink ref="H19" r:id="rId9"/>
+    <hyperlink ref="H20" r:id="rId10"/>
+    <hyperlink ref="H18" r:id="rId11"/>
+    <hyperlink ref="H6" r:id="rId12"/>
+    <hyperlink ref="H7" r:id="rId13"/>
+    <hyperlink ref="H8" r:id="rId14"/>
+    <hyperlink ref="H21" r:id="rId15"/>
+    <hyperlink ref="H29" r:id="rId16"/>
+    <hyperlink ref="H25" r:id="rId17"/>
+    <hyperlink ref="H26" r:id="rId18"/>
+    <hyperlink ref="H36" r:id="rId19"/>
+    <hyperlink ref="H27" r:id="rId20"/>
+    <hyperlink ref="H22" r:id="rId21"/>
+    <hyperlink ref="H23" r:id="rId22"/>
+    <hyperlink ref="H30" r:id="rId23"/>
+    <hyperlink ref="H35" r:id="rId24"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId20"/>
+  <pageSetup orientation="portrait" r:id="rId25"/>
 </worksheet>
 </file>
</xml_diff>